<commit_message>
Adding dish Stirling technology to SSC-TCS interface to SAM. Adding results verification files.
</commit_message>
<xml_diff>
--- a/tcs/Conversion_Coordination/summary table.xlsx
+++ b/tcs/Conversion_Coordination/summary table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="390" windowWidth="19860" windowHeight="13005"/>
+    <workbookView xWindow="735" yWindow="375" windowWidth="19860" windowHeight="13005"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,13 +43,16 @@
     <externalReference r:id="rId32"/>
     <externalReference r:id="rId33"/>
     <externalReference r:id="rId34"/>
+    <externalReference r:id="rId35"/>
+    <externalReference r:id="rId36"/>
+    <externalReference r:id="rId37"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Run description</t>
   </si>
@@ -349,6 +352,39 @@
   </si>
   <si>
     <t xml:space="preserve"> - irradiation basis = Total Horiz.</t>
+  </si>
+  <si>
+    <t>Default run for dish Stirling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cooling fluid = V50%EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cooling fluid = Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cooling fluid = V25%EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cooling fluid = V40%PG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cooling fluid = V40%EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ref cooling fluid = V50%EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ref cooling fluid = Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ref cooling fluid = V25%EG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ref cooling fluid = V40%PG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ref cooling fluid = V40%EG</t>
   </si>
 </sst>
 </file>
@@ -390,7 +426,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +463,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -441,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -492,6 +534,12 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2319,6 +2367,292 @@
         <row r="7">
           <cell r="K7">
             <v>1.5522373012105475E-5</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink32.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="defaults"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="G1">
+            <v>200011.64167050994</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>199952.49516937984</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.9580276595198913E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.6098929605228856E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink33.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="V50%EG"/>
+      <sheetName val="Water"/>
+      <sheetName val="V25%EG"/>
+      <sheetName val="V40%PG"/>
+      <sheetName val="V40%EG"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="G1">
+            <v>200011.64167050994</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>199952.49516937984</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.9580276595198913E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.6098929605228856E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="G1">
+            <v>200311.98681119981</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>200248.96096340005</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-3.1473745230206331E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.4397039535870798E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="G1">
+            <v>200202.87211510984</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>200139.92987788</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-3.1449115260632305E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.4780745054741008E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="G1">
+            <v>199990.00110643997</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>199928.01941561981</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-3.100200312158875E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.4001750080242851E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="G1">
+            <v>200242.71516239038</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>200178.95402316022</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-3.1852069335313525E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.5362627915475519E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink34.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="V50%EG"/>
+      <sheetName val="Water"/>
+      <sheetName val="V25%EG"/>
+      <sheetName val="V40%PG"/>
+      <sheetName val="V40%EG"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="G1">
+            <v>200011.64167050994</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>199952.49516937984</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.9580276595198913E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.6098929605228856E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="G1">
+            <v>202819.18215949956</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>202776.4581059005</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.1069533415335643E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.6006322363675823E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="G1">
+            <v>202122.03713610038</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>202070.69783319999</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.5406604446316612E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.3358541682063286E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="G1">
+            <v>201047.44253334007</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>200989.71455538622</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.8721856778369257E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.3362726349797741E-4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="G1">
+            <v>202499.17984929998</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="G2">
+            <v>202452.2749814</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-2.3168358026251769E-4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="K7">
+            <v>4.7995391764437344E-4</v>
           </cell>
         </row>
       </sheetData>
@@ -3301,11 +3635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F127"/>
+  <dimension ref="A2:F141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C123" sqref="C123"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5630,6 +5964,264 @@
       <c r="F127" s="27">
         <f>'[31]mode = dry bulb'!$G$3</f>
         <v>4.0741297598797891E-6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B129" s="28"/>
+      <c r="C129" s="29">
+        <f>[32]defaults!$G$2</f>
+        <v>199952.49516937984</v>
+      </c>
+      <c r="D129" s="29">
+        <f>[32]defaults!$G$1</f>
+        <v>200011.64167050994</v>
+      </c>
+      <c r="E129" s="30">
+        <f>[32]defaults!$K$7</f>
+        <v>4.6098929605228856E-4</v>
+      </c>
+      <c r="F129" s="31">
+        <f>[32]defaults!$G$3</f>
+        <v>-2.9580276595198913E-4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="28"/>
+      <c r="B130" s="28"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="31"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="28"/>
+      <c r="B131" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C131" s="29">
+        <f>'[33]V50%EG'!$G$2</f>
+        <v>199952.49516937984</v>
+      </c>
+      <c r="D131" s="29">
+        <f>'[33]V50%EG'!$G$1</f>
+        <v>200011.64167050994</v>
+      </c>
+      <c r="E131" s="30">
+        <f>'[33]V50%EG'!$K$7</f>
+        <v>4.6098929605228856E-4</v>
+      </c>
+      <c r="F131" s="31">
+        <f>'[33]V50%EG'!$G$3</f>
+        <v>-2.9580276595198913E-4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="28"/>
+      <c r="B132" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C132" s="29">
+        <f>[33]Water!$G$2</f>
+        <v>200248.96096340005</v>
+      </c>
+      <c r="D132" s="29">
+        <f>[33]Water!$G$1</f>
+        <v>200311.98681119981</v>
+      </c>
+      <c r="E132" s="30">
+        <f>[33]Water!$K$7</f>
+        <v>4.4397039535870798E-4</v>
+      </c>
+      <c r="F132" s="31">
+        <f>[33]Water!$G$3</f>
+        <v>-3.1473745230206331E-4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="28"/>
+      <c r="B133" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C133" s="29">
+        <f>'[33]V25%EG'!$G$2</f>
+        <v>200139.92987788</v>
+      </c>
+      <c r="D133" s="29">
+        <f>'[33]V25%EG'!$G$1</f>
+        <v>200202.87211510984</v>
+      </c>
+      <c r="E133" s="30">
+        <f>'[33]V25%EG'!$K$7</f>
+        <v>4.4780745054741008E-4</v>
+      </c>
+      <c r="F133" s="31">
+        <f>'[33]V25%EG'!$G$3</f>
+        <v>-3.1449115260632305E-4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="28"/>
+      <c r="B134" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C134" s="29">
+        <f>'[33]V40%PG'!$G$2</f>
+        <v>199928.01941561981</v>
+      </c>
+      <c r="D134" s="29">
+        <f>'[33]V40%PG'!$G$1</f>
+        <v>199990.00110643997</v>
+      </c>
+      <c r="E134" s="30">
+        <f>'[33]V40%PG'!$K$7</f>
+        <v>4.4001750080242851E-4</v>
+      </c>
+      <c r="F134" s="31">
+        <f>'[33]V40%PG'!$G$3</f>
+        <v>-3.100200312158875E-4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="28"/>
+      <c r="B135" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C135" s="29">
+        <f>'[33]V40%EG'!$G$2</f>
+        <v>200178.95402316022</v>
+      </c>
+      <c r="D135" s="29">
+        <f>'[33]V40%EG'!$G$1</f>
+        <v>200242.71516239038</v>
+      </c>
+      <c r="E135" s="30">
+        <f>'[33]V40%EG'!$K$7</f>
+        <v>4.5362627915475519E-4</v>
+      </c>
+      <c r="F135" s="31">
+        <f>'[33]V40%EG'!$G$3</f>
+        <v>-3.1852069335313525E-4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="28"/>
+      <c r="B136" s="28"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="28"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="31"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="28"/>
+      <c r="B137" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C137" s="29">
+        <f>'[34]V50%EG'!$G$2</f>
+        <v>199952.49516937984</v>
+      </c>
+      <c r="D137" s="29">
+        <f>'[34]V50%EG'!$G$1</f>
+        <v>200011.64167050994</v>
+      </c>
+      <c r="E137" s="30">
+        <f>'[34]V50%EG'!$K$7</f>
+        <v>4.6098929605228856E-4</v>
+      </c>
+      <c r="F137" s="31">
+        <f>'[34]V50%EG'!$G$3</f>
+        <v>-2.9580276595198913E-4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="28"/>
+      <c r="B138" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C138" s="29">
+        <f>[34]Water!$G$2</f>
+        <v>202776.4581059005</v>
+      </c>
+      <c r="D138" s="29">
+        <f>[34]Water!$G$1</f>
+        <v>202819.18215949956</v>
+      </c>
+      <c r="E138" s="30">
+        <f>[34]Water!$K$7</f>
+        <v>4.6006322363675823E-4</v>
+      </c>
+      <c r="F138" s="31">
+        <f>[34]Water!$G$3</f>
+        <v>-2.1069533415335643E-4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="28"/>
+      <c r="B139" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C139" s="29">
+        <f>'[34]V25%EG'!$G$2</f>
+        <v>202070.69783319999</v>
+      </c>
+      <c r="D139" s="29">
+        <f>'[34]V25%EG'!$G$1</f>
+        <v>202122.03713610038</v>
+      </c>
+      <c r="E139" s="30">
+        <f>'[34]V25%EG'!$K$7</f>
+        <v>4.3358541682063286E-4</v>
+      </c>
+      <c r="F139" s="31">
+        <f>'[34]V25%EG'!$G$3</f>
+        <v>-2.5406604446316612E-4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" s="28"/>
+      <c r="B140" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C140" s="29">
+        <f>'[34]V40%PG'!$G$2</f>
+        <v>200989.71455538622</v>
+      </c>
+      <c r="D140" s="29">
+        <f>'[34]V40%PG'!$G$1</f>
+        <v>201047.44253334007</v>
+      </c>
+      <c r="E140" s="30">
+        <f>'[34]V40%PG'!$K$7</f>
+        <v>4.3362726349797741E-4</v>
+      </c>
+      <c r="F140" s="31">
+        <f>'[34]V40%PG'!$G$3</f>
+        <v>-2.8721856778369257E-4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" s="28"/>
+      <c r="B141" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C141" s="29">
+        <f>'[34]V40%EG'!$G$2</f>
+        <v>202452.2749814</v>
+      </c>
+      <c r="D141" s="29">
+        <f>'[34]V40%EG'!$G$1</f>
+        <v>202499.17984929998</v>
+      </c>
+      <c r="E141" s="30">
+        <f>'[34]V40%EG'!$K$7</f>
+        <v>4.7995391764437344E-4</v>
+      </c>
+      <c r="F141" s="31">
+        <f>'[34]V40%EG'!$G$3</f>
+        <v>-2.3168358026251769E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>